<commit_message>
Copied Files from StudentSenseHat Documentation
</commit_message>
<xml_diff>
--- a/ProposalContentStudentNameRev02.xlsx
+++ b/ProposalContentStudentNameRev02.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{877ACDE8-722C-410D-885A-5CC8B2EE531B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEE92E9-3113-42BB-AF1F-4DA585607F62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Brief description of planned purchases</t>
   </si>
   <si>
-    <t>https://github.com/publicusername/SensorEffector</t>
-  </si>
-  <si>
     <t>Project repository</t>
   </si>
   <si>
@@ -99,20 +96,31 @@
     <t>Thermal and Light Area Monitor</t>
   </si>
   <si>
-    <t>A Paspberry Pi 3 will be purchased as our main circuit board. Aditionally we will purchase theAMG8833 IR THERMAL Camera Breakout to detect human heat signatures, the PCF 8591 Analog to Digital Converter to allow the RPi 3 to read and process the data and to make use of it's photoresistor and finally a BME280 Temp Sensor to provide this information to anyone wanting to use the room and for heating and cooling information.</t>
-  </si>
-  <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>https://github.com/kyelehaynes/N01163090-CENG-317-Project</t>
+  </si>
+  <si>
+    <t>A Raspberry Pi 3 will be purchased as our main circuit board. Aditionally we will purchase theAMG8833 IR THERMAL Camera Breakout to detect human heat signatures, the PCF 8591 Analog to Digital Converter to allow the RPi 3 to read and process the data and to make use of it's photoresistor and finally a BME280 Temp Sensor to provide this information to anyone wanting to use the room and for heating and cooling information.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,10 +143,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -149,8 +158,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,23 +534,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -545,7 +558,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -553,7 +566,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -561,7 +574,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -569,7 +582,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -577,7 +590,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -585,7 +598,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -593,7 +606,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -601,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -609,7 +622,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -617,13 +630,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{DDC452EF-7EA7-4D77-8B97-25A4EF5587A9}"/>
+  </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -702,7 +718,7 @@
         <v>Solution description</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>DataEntry!B1</f>
         <v>43354</v>
@@ -717,7 +733,7 @@
       </c>
       <c r="D2" s="2" t="str">
         <f>DataEntry!B4</f>
-        <v>https://github.com/publicusername/SensorEffector</v>
+        <v>https://github.com/kyelehaynes/N01163090-CENG-317-Project</v>
       </c>
       <c r="E2" s="2" t="str">
         <f>DataEntry!B5</f>
@@ -757,7 +773,7 @@
       </c>
       <c r="N2" s="2" t="str">
         <f>DataEntry!B14</f>
-        <v>A Paspberry Pi 3 will be purchased as our main circuit board. Aditionally we will purchase theAMG8833 IR THERMAL Camera Breakout to detect human heat signatures, the PCF 8591 Analog to Digital Converter to allow the RPi 3 to read and process the data and to make use of it's photoresistor and finally a BME280 Temp Sensor to provide this information to anyone wanting to use the room and for heating and cooling information.</v>
+        <v>A Raspberry Pi 3 will be purchased as our main circuit board. Aditionally we will purchase theAMG8833 IR THERMAL Camera Breakout to detect human heat signatures, the PCF 8591 Analog to Digital Converter to allow the RPi 3 to read and process the data and to make use of it's photoresistor and finally a BME280 Temp Sensor to provide this information to anyone wanting to use the room and for heating and cooling information.</v>
       </c>
       <c r="O2" s="2" t="str">
         <f>DataEntry!B15</f>

</xml_diff>